<commit_message>
working on sonification_citation_analysis.ipynb, seems to be basically working but can not get colours in graph to be correct and need to optimise community algorithm when data is large
</commit_message>
<xml_diff>
--- a/data/fake/citation_data_fake_prep.xlsx
+++ b/data/fake/citation_data_fake_prep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/nch169_newcastle_ac_uk/Documents/work/sonification_research/sonic_intangibles/si_citationAnalysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/nch169_newcastle_ac_uk/Documents/work/sonification_research/sonic_intangibles/si_citationAnalysis/data/fake/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{C19A9AE5-DBE8-084F-A686-68B67D5EFAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1281B8D-623B-0242-ACBA-718477F7FF14}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{C19A9AE5-DBE8-084F-A686-68B67D5EFAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5CABCAA-7F74-C749-8289-0665F7DF12AB}"/>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="5760" windowWidth="27640" windowHeight="16680" xr2:uid="{9909D332-0698-EE43-B568-BE5B72009470}"/>
+    <workbookView xWindow="8200" yWindow="-21000" windowWidth="27640" windowHeight="16680" xr2:uid="{9909D332-0698-EE43-B568-BE5B72009470}"/>
   </bookViews>
   <sheets>
     <sheet name="citation_data_fake_prep" sheetId="1" r:id="rId1"/>
@@ -141,32 +141,34 @@
     <t>WOS:000274369800014</t>
   </si>
   <si>
-    <t>Group 3</t>
-  </si>
-  <si>
-    <t>Group 4</t>
-  </si>
-  <si>
-    <t>Group 5</t>
-  </si>
-  <si>
-    <t>Group 1 (well connected)</t>
-  </si>
-  <si>
-    <t>Group 2 (isolated, except one link)</t>
-  </si>
-  <si>
     <t>Highly Citation paper by all groups</t>
   </si>
   <si>
     <t>Total Papers:</t>
+  </si>
+  <si>
+    <t>Group 3 (N=5)</t>
+  </si>
+  <si>
+    <t>Group 4 (N=4)</t>
+  </si>
+  <si>
+    <t>Group 5 (N=4)</t>
+  </si>
+  <si>
+    <t>Group 2 (isolated, except one link) 
+N=6)</t>
+  </si>
+  <si>
+    <t>Group 1 (well connected)
+N=7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -336,6 +338,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -678,7 +686,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -689,6 +697,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1066,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CF3F2A-E2F6-9349-97EA-77FF781B373F}">
   <dimension ref="A1:Q153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1083,8 +1095,8 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>31</v>
+      <c r="I1" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -1093,7 +1105,7 @@
         <v>2</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="Q1" t="str" cm="1">
         <f t="array" ref="Q1:Q27">_xlfn.UNIQUE(B2:B19999)</f>
@@ -1215,8 +1227,8 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>32</v>
+      <c r="I8" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>9</v>
@@ -1326,7 +1338,7 @@
         <v>6</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>15</v>
@@ -1418,7 +1430,7 @@
         <v>4</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J19" t="s">
         <v>20</v>
@@ -1492,7 +1504,7 @@
         <v>7</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>24</v>
@@ -1588,7 +1600,7 @@
         <v>6</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="J29" s="6">
         <f xml:space="preserve"> COUNTIF(L2:L26,"*")</f>
@@ -1603,215 +1615,241 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B32" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B33" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B41" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B42" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B43" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B49" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B50" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B51" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I51" s="9"/>
+    </row>
+    <row r="52" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B52" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B53" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B56" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I56" s="9"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>9</v>
       </c>
@@ -1819,7 +1857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>9</v>
       </c>
@@ -1827,7 +1865,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>9</v>
       </c>
@@ -1835,7 +1873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>10</v>
       </c>
@@ -1843,7 +1881,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>10</v>
       </c>
@@ -1851,7 +1889,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>10</v>
       </c>
@@ -1859,7 +1897,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>10</v>
       </c>
@@ -1867,7 +1905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>11</v>
       </c>

</xml_diff>